<commit_message>
scoreboard_matrix and backend stuff
Getting ready for new stuff
</commit_message>
<xml_diff>
--- a/csv/game states.xlsx
+++ b/csv/game states.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8b29edc4376667/Projects/Python/MLB-Stats/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{872CC6C0-7F4F-4023-BEF8-A042F53196A4}"/>
+  <xr:revisionPtr revIDLastSave="342" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85184A4A-3B84-4659-87D4-9FC9F7B76A7E}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
   </bookViews>
   <sheets>
     <sheet name="nonsortable" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>abstractGameState</t>
   </si>
@@ -339,6 +339,24 @@
   </si>
   <si>
     <t>bees? Drying/preping field?</t>
+  </si>
+  <si>
+    <t>Umpire review: Tag play</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>detailedState literally blank. Rangers shift challenge and Rays too many mound visits 5/20</t>
+  </si>
+  <si>
+    <t>Manager challenge: Fan Interference</t>
+  </si>
+  <si>
+    <t>MN</t>
   </si>
 </sst>
 </file>
@@ -712,11 +730,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,10 +997,10 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,10 +1008,10 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="2" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,10 +1019,10 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,10 +1030,10 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="2" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,10 +1041,10 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1034,10 +1052,10 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1045,56 +1063,56 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
+      <c r="D27" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C28" s="5"/>
       <c r="E28" s="2" t="s">
-        <v>54</v>
+        <v>102</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1102,98 +1120,93 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>28</v>
+      <c r="C32" s="5"/>
+      <c r="D32" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="6"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="E33" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="2" t="s">
-        <v>67</v>
+      <c r="C35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>92</v>
+        <v>17</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1204,20 +1217,23 @@
         <v>67</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>77</v>
+        <v>10</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>64</v>
+        <v>10</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,40 +1241,75 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="2" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F36" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
+  <autoFilter ref="A1:F39" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
   <mergeCells count="14">
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A9:A33"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C13:C27"/>
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B9:B33"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B9:B36"/>
     <mergeCell ref="C3:C9"/>
     <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B37:B44"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="A9:A36"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C13:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
scoreboard_matrix reduced data GET requests
no longer sending empty GET requests to the ESP32. I was only sending data the ESP was looking for but the check for whether or not their was data was checking all attributes and not the ones the ESP cared about
</commit_message>
<xml_diff>
--- a/csv/game states.xlsx
+++ b/csv/game states.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8b29edc4376667/Projects/Python/MLB-Stats/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="345" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C03CDF6C-979A-46D1-8FC8-126DE7A3310E}"/>
+  <xr:revisionPtr revIDLastSave="358" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25F13948-B53D-48F9-BC46-497E550B7DE5}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
   </bookViews>
   <sheets>
     <sheet name="nonsortable" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
   <si>
     <t>abstractGameState</t>
   </si>
@@ -363,6 +363,24 @@
   </si>
   <si>
     <t>MD</t>
+  </si>
+  <si>
+    <t>Completed Early</t>
+  </si>
+  <si>
+    <t>OO</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>Futures Game (7 inning game)</t>
+  </si>
+  <si>
+    <t>Umpire review: Hit by pitch</t>
+  </si>
+  <si>
+    <t>NI</t>
   </si>
 </sst>
 </file>
@@ -433,10 +451,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,11 +750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,10 +1173,10 @@
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="2" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,87 +1184,85 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="2" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>28</v>
+      <c r="C36" s="5"/>
+      <c r="D36" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="2" t="s">
+      <c r="D38" s="6"/>
+      <c r="E38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="2" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,34 +1270,37 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="2" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>69</v>
+        <v>10</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>77</v>
+      <c r="C43" s="5"/>
+      <c r="D43" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1293,40 +1308,78 @@
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="2" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>75</v>
+        <v>110</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F40" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
+  <autoFilter ref="A1:F42" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
   <mergeCells count="14">
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="A9:A37"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C13:C30"/>
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B9:B37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B9:B38"/>
     <mergeCell ref="C3:C9"/>
     <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="B39:B48"/>
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="A9:A38"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C13:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Matchup keyward error bodge
</commit_message>
<xml_diff>
--- a/csv/game states.xlsx
+++ b/csv/game states.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8b29edc4376667/Projects/Python/MLB-Stats/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25F13948-B53D-48F9-BC46-497E550B7DE5}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6041111F-0DC6-4C31-A116-98ECBE51D119}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
   </bookViews>
   <sheets>
     <sheet name="nonsortable" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="116">
   <si>
     <t>abstractGameState</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>NI</t>
+  </si>
+  <si>
+    <t>Umpire review: Record keeping</t>
+  </si>
+  <si>
+    <t>NK</t>
   </si>
 </sst>
 </file>
@@ -451,6 +457,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -750,11 +760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,10 +1194,10 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="2" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1195,74 +1205,71 @@
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="2" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>28</v>
+      <c r="C37" s="5"/>
+      <c r="D37" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="2" t="s">
+      <c r="D39" s="6"/>
+      <c r="E39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1270,37 +1277,40 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>68</v>
+        <v>109</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C42" s="5"/>
       <c r="D42" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>92</v>
+        <v>10</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1308,13 +1318,10 @@
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1322,64 +1329,78 @@
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>69</v>
+        <v>110</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>77</v>
+      <c r="C46" s="5"/>
+      <c r="D46" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="2" t="s">
-        <v>76</v>
+      <c r="C47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F42" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
+  <autoFilter ref="A1:F43" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
   <mergeCells count="14">
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="B40:B49"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A9:A39"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C13:C30"/>
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B9:B38"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B9:B39"/>
     <mergeCell ref="C3:C9"/>
     <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="B39:B48"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="A9:A38"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C13:C30"/>
+    <mergeCell ref="C31:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new game state: OT
</commit_message>
<xml_diff>
--- a/csv/game states.xlsx
+++ b/csv/game states.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8b29edc4376667/Projects/Python/at_bat/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDE08C15-0535-4192-9B39-0DB6EEE1708E}"/>
+  <xr:revisionPtr revIDLastSave="421" documentId="8_{1E7C1C6B-8C31-4479-B74A-66C136A4727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A0C74FE-86B6-4C81-A24D-E797EDC25FC0}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{F5CA1E43-766A-4086-8122-BB1D980A4810}"/>
   </bookViews>
   <sheets>
     <sheet name="nonsortable" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonsortable!$A$1:$F$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="143">
   <si>
     <t>abstractGameState</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>MJ</t>
+  </si>
+  <si>
+    <t>Game Over: Tied</t>
+  </si>
+  <si>
+    <t>OT</t>
   </si>
 </sst>
 </file>
@@ -512,10 +518,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,11 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -872,10 +878,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -889,9 +895,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -905,9 +911,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
         <v>71</v>
       </c>
@@ -916,9 +922,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>95</v>
       </c>
@@ -927,9 +933,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
         <v>93</v>
       </c>
@@ -941,9 +947,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
@@ -952,9 +958,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="2" t="s">
         <v>69</v>
       </c>
@@ -963,13 +969,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -981,9 +987,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -994,9 +1000,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1005,9 +1011,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1019,9 +1025,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1032,9 +1038,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2" t="s">
         <v>129</v>
       </c>
@@ -1046,9 +1052,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
@@ -1057,9 +1063,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="2" t="s">
         <v>104</v>
       </c>
@@ -1068,9 +1074,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="2" t="s">
         <v>55</v>
       </c>
@@ -1079,9 +1085,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1090,9 +1096,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1101,9 +1107,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
@@ -1112,9 +1118,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
@@ -1123,9 +1129,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="2" t="s">
         <v>139</v>
       </c>
@@ -1134,9 +1140,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="2" t="s">
         <v>123</v>
       </c>
@@ -1145,9 +1151,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="2" t="s">
         <v>102</v>
       </c>
@@ -1156,9 +1162,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="2" t="s">
         <v>87</v>
       </c>
@@ -1167,9 +1173,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1178,9 +1184,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="2" t="s">
         <v>77</v>
       </c>
@@ -1189,9 +1195,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="2" t="s">
         <v>57</v>
       </c>
@@ -1200,9 +1206,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="2" t="s">
         <v>49</v>
       </c>
@@ -1211,9 +1217,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="2" t="s">
         <v>59</v>
       </c>
@@ -1222,9 +1228,9 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
@@ -1233,9 +1239,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="E32" s="2" t="s">
         <v>100</v>
       </c>
@@ -1244,9 +1250,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="2" t="s">
         <v>114</v>
       </c>
@@ -1258,9 +1264,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
       <c r="E34" s="2" t="s">
         <v>81</v>
       </c>
@@ -1269,9 +1275,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1282,9 +1288,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="2" t="s">
         <v>121</v>
       </c>
@@ -1293,9 +1299,9 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
@@ -1304,9 +1310,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="2" t="s">
         <v>91</v>
       </c>
@@ -1315,9 +1321,9 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="2" t="s">
         <v>110</v>
       </c>
@@ -1326,9 +1332,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="2" t="s">
         <v>112</v>
       </c>
@@ -1337,9 +1343,9 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
       <c r="D41" s="2" t="s">
         <v>85</v>
       </c>
@@ -1348,9 +1354,9 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
       <c r="D42" s="2" t="s">
         <v>119</v>
       </c>
@@ -1359,9 +1365,9 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
       <c r="D43" s="2" t="s">
         <v>25</v>
       </c>
@@ -1370,9 +1376,9 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
       <c r="D44" s="2" t="s">
         <v>117</v>
       </c>
@@ -1381,12 +1387,12 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -1395,25 +1401,25 @@
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="6"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -1427,9 +1433,9 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
       <c r="D48" s="2" t="s">
         <v>106</v>
       </c>
@@ -1441,9 +1447,9 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
       <c r="D49" s="2" t="s">
         <v>65</v>
       </c>
@@ -1452,164 +1458,178 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="2" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="2" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="2" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="2" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="2" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="4" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D59" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="1"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="2" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="1"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="2" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F50" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
+  <autoFilter ref="A1:F51" xr:uid="{8B849384-B473-4938-862B-0224328C5BC9}"/>
   <mergeCells count="16">
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="B47:B60"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="A9:A46"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C13:C34"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="A47:A58"/>
-    <mergeCell ref="C50:C54"/>
-    <mergeCell ref="C58:C60"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="D45:D46"/>
     <mergeCell ref="B9:B46"/>
     <mergeCell ref="C3:C9"/>
     <mergeCell ref="B2:B8"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="B47:B61"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="A9:A46"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C34"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="A47:A59"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C47:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>